<commit_message>
Complete select testsuit to Run from excel file
</commit_message>
<xml_diff>
--- a/testSElenium/Data_Main.xlsx
+++ b/testSElenium/Data_Main.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dnguyen4\Documents\Script_Tool-_JAZZ\testSElenium\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pdo2\Desktop\Script Tool\Src\testSElenium\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{55F44447-D2ED-41F7-BA8C-3F9A3AB4FDF7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{757B62C6-E99F-4850-987B-165E92EA8695}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data_Main" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>Num</t>
   </si>
@@ -41,9 +41,6 @@
   </si>
   <si>
     <t>CommandlineTest - Load configuration with Script Formatting from PC_Matrix M300N</t>
-  </si>
-  <si>
-    <t>None</t>
   </si>
   <si>
     <t>CommandlineTest - Verify simulator M300N_Matrix M300N</t>
@@ -70,7 +67,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -904,7 +901,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -914,7 +911,7 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="78.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -949,7 +946,7 @@
         <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F2" t="b">
         <v>1</v>
@@ -963,10 +960,10 @@
         <v>244407</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="F3" t="b">
         <v>1</v>
@@ -980,10 +977,10 @@
         <v>244405</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F4" t="b">
         <v>0</v>
@@ -997,10 +994,10 @@
         <v>244403</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D5" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="F5" t="b">
         <v>1</v>
@@ -1014,10 +1011,10 @@
         <v>244401</v>
       </c>
       <c r="C6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" t="s">
         <v>12</v>
-      </c>
-      <c r="D6" t="s">
-        <v>11</v>
       </c>
       <c r="F6" t="b">
         <v>0</v>
@@ -1025,7 +1022,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D6" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"TestExecute-PC,TestComplete14_,TEST02-PC, None"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Check Run complete (done)
</commit_message>
<xml_diff>
--- a/testSElenium/Data_Main.xlsx
+++ b/testSElenium/Data_Main.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pdo2\Desktop\Script Tool\Src\testSElenium\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{360C24EA-6C8A-4ED0-8FB2-A47BC5D8E0F2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05741551-A466-4676-96F1-813BAF46EEC1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>Num</t>
   </si>
@@ -53,6 +53,9 @@
   </si>
   <si>
     <t>CommandlineTest - Verify simulator M300N 772-010_Matrix M300N</t>
+  </si>
+  <si>
+    <t>TEST02-PC</t>
   </si>
   <si>
     <t>CommandlineTest - Verify simulator XRF_Matrix M300N</t>
@@ -943,7 +946,7 @@
         <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F2" t="b">
         <v>1</v>
@@ -960,7 +963,7 @@
         <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="F3" t="b">
         <v>1</v>
@@ -1008,7 +1011,7 @@
         <v>244401</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D6" t="s">
         <v>7</v>

</xml_diff>